<commit_message>
made seperate folder for no cell filtering preprocessing figs
</commit_message>
<xml_diff>
--- a/sample_list.xlsx
+++ b/sample_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randymi\Desktop\seuratwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150489D6-11B3-41CF-992D-98E562DA56A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6B9E87-C41E-44D7-B0F4-EF78393253BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,12 +467,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -502,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,6 +518,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,7 +827,7 @@
   <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -848,160 +858,160 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
@@ -1156,52 +1166,52 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
@@ -1220,144 +1230,144 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="C23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="C28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="C29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">

</xml_diff>

<commit_message>
finished mapping ensembl id to symbols. Initial dotplot
</commit_message>
<xml_diff>
--- a/sample_list.xlsx
+++ b/sample_list.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randymi\Desktop\seuratwork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AFF335A-1077-414E-8D8F-F827A9D14A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="44265" yWindow="5085" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="mQ8rQ1de4+Gu3TxmkFXJjZVDeMIsMKimAfFr/nJ2BJE="/>
@@ -420,34 +429,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -455,7 +469,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -465,7 +479,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -479,44 +499,46 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -706,27 +728,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.86"/>
-    <col customWidth="1" min="2" max="2" width="19.71"/>
-    <col customWidth="1" min="3" max="5" width="8.71"/>
-    <col customWidth="1" min="6" max="6" width="36.57"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="22.86328125" customWidth="1"/>
+    <col min="2" max="2" width="19.73046875" customWidth="1"/>
+    <col min="3" max="5" width="8.73046875" customWidth="1"/>
+    <col min="6" max="6" width="36.53125" customWidth="1"/>
+    <col min="7" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -768,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -787,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -808,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
@@ -829,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -850,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -871,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -892,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -913,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -932,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -953,7 +977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -974,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -995,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1016,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1062,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1108,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
@@ -1127,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1146,7 +1170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1184,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>39</v>
       </c>
@@ -1205,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
@@ -1226,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
@@ -1247,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -1268,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
@@ -1287,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>39</v>
       </c>
@@ -1306,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>39</v>
       </c>
@@ -1348,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>39</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1386,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
+    <row r="33" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -1405,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="34" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -1424,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1443,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -1481,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
@@ -1500,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1519,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -1538,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1557,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1576,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -1595,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1614,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" ht="14.25" customHeight="1">
+    <row r="45" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
@@ -1633,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" ht="14.25" customHeight="1">
+    <row r="46" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" ht="14.25" customHeight="1">
+    <row r="47" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>39</v>
       </c>
@@ -1671,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" ht="14.25" customHeight="1">
+    <row r="48" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
@@ -1690,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="49" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
@@ -1709,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" ht="14.25" customHeight="1">
+    <row r="50" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>39</v>
       </c>
@@ -1728,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>39</v>
       </c>
@@ -1747,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" ht="14.25" customHeight="1">
+    <row r="52" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>39</v>
       </c>
@@ -1766,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>39</v>
       </c>
@@ -1785,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>39</v>
       </c>
@@ -1804,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="2" t="s">
         <v>39</v>
       </c>
@@ -1823,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>39</v>
       </c>
@@ -1842,7 +1866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>39</v>
       </c>
@@ -1861,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
@@ -1880,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" ht="14.25" customHeight="1">
+    <row r="59" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>77</v>
       </c>
@@ -1901,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" ht="14.25" customHeight="1">
+    <row r="60" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>77</v>
       </c>
@@ -1922,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" ht="14.25" customHeight="1">
+    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="2" t="s">
         <v>77</v>
       </c>
@@ -1943,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" ht="14.25" customHeight="1">
+    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="2" t="s">
         <v>77</v>
       </c>
@@ -1964,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="2" t="s">
         <v>83</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="2" t="s">
         <v>83</v>
       </c>
@@ -2006,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="2" t="s">
         <v>83</v>
       </c>
@@ -2027,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="2" t="s">
         <v>83</v>
       </c>
@@ -2048,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="2" t="s">
         <v>83</v>
       </c>
@@ -2069,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>83</v>
       </c>
@@ -2090,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -2111,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="2" t="s">
         <v>83</v>
       </c>
@@ -2132,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="2" t="s">
         <v>83</v>
       </c>
@@ -2153,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="2" t="s">
         <v>93</v>
       </c>
@@ -2174,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="2" t="s">
         <v>93</v>
       </c>
@@ -2195,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1">
+    <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="2" t="s">
         <v>93</v>
       </c>
@@ -2216,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" ht="14.25" customHeight="1">
+    <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="2" t="s">
         <v>93</v>
       </c>
@@ -2237,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>93</v>
       </c>
@@ -2258,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1">
+    <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>93</v>
       </c>
@@ -2279,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" ht="14.25" customHeight="1">
+    <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="2" t="s">
         <v>93</v>
       </c>
@@ -2300,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="2" t="s">
         <v>93</v>
       </c>
@@ -2321,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>93</v>
       </c>
@@ -2342,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>93</v>
       </c>
@@ -2363,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>93</v>
       </c>
@@ -2384,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>93</v>
       </c>
@@ -2405,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>93</v>
       </c>
@@ -2426,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>93</v>
       </c>
@@ -2447,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>111</v>
       </c>
@@ -2468,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" ht="14.25" customHeight="1">
+    <row r="87" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>111</v>
       </c>
@@ -2489,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" ht="14.25" customHeight="1">
+    <row r="88" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="2" t="s">
         <v>111</v>
       </c>
@@ -2510,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" ht="14.25" customHeight="1">
+    <row r="89" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="2" t="s">
         <v>111</v>
       </c>
@@ -2531,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" ht="14.25" customHeight="1">
+    <row r="90" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
         <v>111</v>
       </c>
@@ -2552,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="91" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
         <v>111</v>
       </c>
@@ -2573,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
         <v>111</v>
       </c>
@@ -2594,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>111</v>
       </c>
@@ -2615,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
         <v>111</v>
       </c>
@@ -2636,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="2" t="s">
         <v>111</v>
       </c>
@@ -2657,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="2" t="s">
         <v>111</v>
       </c>
@@ -2678,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
         <v>111</v>
       </c>
@@ -2699,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
         <v>111</v>
       </c>
@@ -2720,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" ht="14.25" customHeight="1">
+    <row r="99" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
         <v>111</v>
       </c>
@@ -2741,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" ht="14.25" customHeight="1">
+    <row r="100" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="2" t="s">
         <v>111</v>
       </c>
@@ -2762,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" ht="14.25" customHeight="1">
+    <row r="101" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="2" t="s">
         <v>111</v>
       </c>
@@ -2783,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" ht="14.25" customHeight="1">
+    <row r="102" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="2" t="s">
         <v>111</v>
       </c>
@@ -2804,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" ht="14.25" customHeight="1">
+    <row r="103" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="2" t="s">
         <v>111</v>
       </c>
@@ -2825,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" ht="14.25" customHeight="1">
+    <row r="104" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="2" t="s">
         <v>111</v>
       </c>
@@ -2846,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" ht="14.25" customHeight="1">
+    <row r="105" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
         <v>111</v>
       </c>
@@ -2867,901 +2891,901 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="106" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="108" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="110" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="112" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="A1:A1000">
     <cfRule type="colorScale" priority="1">
@@ -3774,8 +3798,6 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1000">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3787,9 +3809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started HS doublet redo
</commit_message>
<xml_diff>
--- a/sample_list.xlsx
+++ b/sample_list.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randymi\Desktop\seuratwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CBF841-D496-46E5-B40D-C11845A4F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3FEEE9-324B-404B-8CB0-BDD021A74835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" r:id="rId1"/>
     <sheet name="key" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">samples!$A$1:$Q$106</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -119,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="259">
   <si>
     <t>GSE</t>
   </si>
@@ -886,9 +889,6 @@
     <t>HS_data_expanded_2  = Red + Yellow</t>
   </si>
   <si>
-    <t>Haniffa</t>
-  </si>
-  <si>
     <t>Proportion Nan Cluster Label</t>
   </si>
   <si>
@@ -896,6 +896,9 @@
   </si>
   <si>
     <t>GSM Post QC Cell Count</t>
+  </si>
+  <si>
+    <t>haniffa_hs7</t>
   </si>
 </sst>
 </file>
@@ -944,6 +947,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1026,7 +1030,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1108,7 +1112,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1374,11 +1377,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106:D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1420,13 +1424,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>6</v>
@@ -1496,7 +1500,7 @@
         <v>42.22</v>
       </c>
       <c r="P2" s="12">
-        <f>14/5</f>
+        <f t="shared" ref="P2:P10" si="0">14/5</f>
         <v>2.8</v>
       </c>
       <c r="Q2" s="5"/>
@@ -1544,7 +1548,7 @@
         <v>42.22</v>
       </c>
       <c r="P3" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q3" s="5"/>
@@ -1592,7 +1596,7 @@
         <v>42.22</v>
       </c>
       <c r="P4" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q4" s="5"/>
@@ -1638,7 +1642,7 @@
         <v>42.22</v>
       </c>
       <c r="P5" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q5" s="5"/>
@@ -1686,7 +1690,7 @@
         <v>42.22</v>
       </c>
       <c r="P6" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q6" s="5"/>
@@ -1732,7 +1736,7 @@
         <v>42.22</v>
       </c>
       <c r="P7" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q7" s="5"/>
@@ -1778,7 +1782,7 @@
         <v>42.22</v>
       </c>
       <c r="P8" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q8" s="5"/>
@@ -1826,7 +1830,7 @@
         <v>42.22</v>
       </c>
       <c r="P9" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q9" s="5"/>
@@ -1874,7 +1878,7 @@
         <v>42.22</v>
       </c>
       <c r="P10" s="12">
-        <f>14/5</f>
+        <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
       <c r="Q10" s="5"/>
@@ -2047,7 +2051,7 @@
       <c r="P14" s="14"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -2080,7 +2084,7 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -2113,7 +2117,7 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -2148,7 +2152,7 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
         <v>34</v>
       </c>
@@ -2663,7 +2667,7 @@
       <c r="P30" s="14"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="8" t="s">
         <v>39</v>
       </c>
@@ -2698,7 +2702,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="8" t="s">
         <v>39</v>
       </c>
@@ -2733,7 +2737,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="8" t="s">
         <v>39</v>
       </c>
@@ -2768,7 +2772,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="8" t="s">
         <v>39</v>
       </c>
@@ -2803,7 +2807,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="8" t="s">
         <v>39</v>
       </c>
@@ -2838,7 +2842,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="8" t="s">
         <v>39</v>
       </c>
@@ -2873,7 +2877,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="8" t="s">
         <v>39</v>
       </c>
@@ -2908,7 +2912,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="8" t="s">
         <v>39</v>
       </c>
@@ -2943,7 +2947,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="8" t="s">
         <v>39</v>
       </c>
@@ -2978,7 +2982,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
         <v>39</v>
       </c>
@@ -3013,7 +3017,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="8" t="s">
         <v>39</v>
       </c>
@@ -3048,7 +3052,7 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
         <v>39</v>
       </c>
@@ -3083,7 +3087,7 @@
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="8" t="s">
         <v>39</v>
       </c>
@@ -3118,7 +3122,7 @@
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="8" t="s">
         <v>39</v>
       </c>
@@ -3153,7 +3157,7 @@
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="8" t="s">
         <v>39</v>
       </c>
@@ -3188,7 +3192,7 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="8" t="s">
         <v>39</v>
       </c>
@@ -3223,7 +3227,7 @@
       <c r="P46" s="5"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="8" t="s">
         <v>39</v>
       </c>
@@ -3258,7 +3262,7 @@
       <c r="P47" s="5"/>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="8" t="s">
         <v>39</v>
       </c>
@@ -3293,7 +3297,7 @@
       <c r="P48" s="5"/>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="8" t="s">
         <v>39</v>
       </c>
@@ -3328,7 +3332,7 @@
       <c r="P49" s="5"/>
       <c r="Q49" s="5"/>
     </row>
-    <row r="50" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
         <v>39</v>
       </c>
@@ -3363,7 +3367,7 @@
       <c r="P50" s="5"/>
       <c r="Q50" s="5"/>
     </row>
-    <row r="51" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="8" t="s">
         <v>39</v>
       </c>
@@ -3398,7 +3402,7 @@
       <c r="P51" s="5"/>
       <c r="Q51" s="5"/>
     </row>
-    <row r="52" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="8" t="s">
         <v>39</v>
       </c>
@@ -3433,7 +3437,7 @@
       <c r="P52" s="5"/>
       <c r="Q52" s="5"/>
     </row>
-    <row r="53" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="8" t="s">
         <v>39</v>
       </c>
@@ -3468,7 +3472,7 @@
       <c r="P53" s="5"/>
       <c r="Q53" s="5"/>
     </row>
-    <row r="54" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="8" t="s">
         <v>39</v>
       </c>
@@ -3503,7 +3507,7 @@
       <c r="P54" s="5"/>
       <c r="Q54" s="5"/>
     </row>
-    <row r="55" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>39</v>
       </c>
@@ -3538,7 +3542,7 @@
       <c r="P55" s="5"/>
       <c r="Q55" s="5"/>
     </row>
-    <row r="56" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="8" t="s">
         <v>39</v>
       </c>
@@ -3573,7 +3577,7 @@
       <c r="P56" s="5"/>
       <c r="Q56" s="5"/>
     </row>
-    <row r="57" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="8" t="s">
         <v>39</v>
       </c>
@@ -3608,7 +3612,7 @@
       <c r="P57" s="5"/>
       <c r="Q57" s="5"/>
     </row>
-    <row r="58" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
         <v>39</v>
       </c>
@@ -3643,7 +3647,7 @@
       <c r="P58" s="5"/>
       <c r="Q58" s="5"/>
     </row>
-    <row r="59" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="8" t="s">
         <v>77</v>
       </c>
@@ -3676,7 +3680,7 @@
       <c r="P59" s="5"/>
       <c r="Q59" s="5"/>
     </row>
-    <row r="60" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="8" t="s">
         <v>77</v>
       </c>
@@ -3709,7 +3713,7 @@
       <c r="P60" s="5"/>
       <c r="Q60" s="5"/>
     </row>
-    <row r="61" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="8" t="s">
         <v>77</v>
       </c>
@@ -3742,7 +3746,7 @@
       <c r="P61" s="5"/>
       <c r="Q61" s="5"/>
     </row>
-    <row r="62" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="8" t="s">
         <v>77</v>
       </c>
@@ -3910,7 +3914,7 @@
       <c r="P65" s="5"/>
       <c r="Q65" s="5"/>
     </row>
-    <row r="66" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="8" t="s">
         <v>83</v>
       </c>
@@ -3943,7 +3947,7 @@
       <c r="P66" s="5"/>
       <c r="Q66" s="5"/>
     </row>
-    <row r="67" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="8" t="s">
         <v>83</v>
       </c>
@@ -3976,7 +3980,7 @@
       <c r="P67" s="5"/>
       <c r="Q67" s="5"/>
     </row>
-    <row r="68" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="8" t="s">
         <v>83</v>
       </c>
@@ -4009,7 +4013,7 @@
       <c r="P68" s="5"/>
       <c r="Q68" s="5"/>
     </row>
-    <row r="69" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="8" t="s">
         <v>83</v>
       </c>
@@ -4042,7 +4046,7 @@
       <c r="P69" s="5"/>
       <c r="Q69" s="5"/>
     </row>
-    <row r="70" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="8" t="s">
         <v>83</v>
       </c>
@@ -4075,7 +4079,7 @@
       <c r="P70" s="5"/>
       <c r="Q70" s="5"/>
     </row>
-    <row r="71" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="8" t="s">
         <v>83</v>
       </c>
@@ -4462,7 +4466,7 @@
       <c r="P79" s="5"/>
       <c r="Q79" s="5"/>
     </row>
-    <row r="80" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="8" t="s">
         <v>93</v>
       </c>
@@ -4495,7 +4499,7 @@
       <c r="P80" s="5"/>
       <c r="Q80" s="5"/>
     </row>
-    <row r="81" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="8" t="s">
         <v>93</v>
       </c>
@@ -4528,7 +4532,7 @@
       <c r="P81" s="5"/>
       <c r="Q81" s="5"/>
     </row>
-    <row r="82" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="8" t="s">
         <v>93</v>
       </c>
@@ -4561,7 +4565,7 @@
       <c r="P82" s="5"/>
       <c r="Q82" s="5"/>
     </row>
-    <row r="83" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="8" t="s">
         <v>93</v>
       </c>
@@ -4594,7 +4598,7 @@
       <c r="P83" s="5"/>
       <c r="Q83" s="5"/>
     </row>
-    <row r="84" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="8" t="s">
         <v>93</v>
       </c>
@@ -4627,7 +4631,7 @@
       <c r="P84" s="5"/>
       <c r="Q84" s="5"/>
     </row>
-    <row r="85" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
         <v>93</v>
       </c>
@@ -5110,7 +5114,7 @@
       <c r="P95" s="5"/>
       <c r="Q95" s="5"/>
     </row>
-    <row r="96" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="8" t="s">
         <v>111</v>
       </c>
@@ -5143,7 +5147,7 @@
       <c r="P96" s="5"/>
       <c r="Q96" s="5"/>
     </row>
-    <row r="97" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="8" t="s">
         <v>111</v>
       </c>
@@ -5176,7 +5180,7 @@
       <c r="P97" s="5"/>
       <c r="Q97" s="5"/>
     </row>
-    <row r="98" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="8" t="s">
         <v>111</v>
       </c>
@@ -5209,7 +5213,7 @@
       <c r="P98" s="5"/>
       <c r="Q98" s="5"/>
     </row>
-    <row r="99" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="8" t="s">
         <v>111</v>
       </c>
@@ -5242,7 +5246,7 @@
       <c r="P99" s="5"/>
       <c r="Q99" s="5"/>
     </row>
-    <row r="100" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="8" t="s">
         <v>111</v>
       </c>
@@ -5275,7 +5279,7 @@
       <c r="P100" s="5"/>
       <c r="Q100" s="5"/>
     </row>
-    <row r="101" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="8" t="s">
         <v>111</v>
       </c>
@@ -5308,7 +5312,7 @@
       <c r="P101" s="5"/>
       <c r="Q101" s="5"/>
     </row>
-    <row r="102" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="8" t="s">
         <v>111</v>
       </c>
@@ -5341,7 +5345,7 @@
       <c r="P102" s="5"/>
       <c r="Q102" s="5"/>
     </row>
-    <row r="103" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="8" t="s">
         <v>111</v>
       </c>
@@ -5374,7 +5378,7 @@
       <c r="P103" s="5"/>
       <c r="Q103" s="5"/>
     </row>
-    <row r="104" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="8" t="s">
         <v>111</v>
       </c>
@@ -5407,7 +5411,7 @@
       <c r="P104" s="5"/>
       <c r="Q104" s="5"/>
     </row>
-    <row r="105" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="8" t="s">
         <v>111</v>
       </c>
@@ -5442,10 +5446,10 @@
     </row>
     <row r="106" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B106" s="5">
-        <v>0</v>
+        <v>258</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>258</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>9</v>
@@ -5458,10 +5462,10 @@
       <c r="G106" s="37">
         <v>1.83920126116657E-2</v>
       </c>
-      <c r="H106" s="39">
+      <c r="H106">
         <v>5709</v>
       </c>
-      <c r="I106" s="39">
+      <c r="I106">
         <v>105</v>
       </c>
       <c r="J106" s="5" t="b">
@@ -6373,6 +6377,13 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
+  <autoFilter ref="A1:Q106" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q1000">
     <sortCondition ref="A1:A1000"/>
   </sortState>

</xml_diff>